<commit_message>
added the appendix analyses
</commit_message>
<xml_diff>
--- a/data/GI.data/MasterGI.TRCA.xlsx
+++ b/data/GI.data/MasterGI.TRCA.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4039" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4127" uniqueCount="749">
   <si>
     <t>lon</t>
   </si>
@@ -2187,9 +2187,6 @@
     <t>latitude determine using Google maps from the street address</t>
   </si>
   <si>
-    <t>Whether the data is available to be share publically</t>
-  </si>
-  <si>
     <t>The location from where the data was retrieved from</t>
   </si>
   <si>
@@ -2206,6 +2203,75 @@
   </si>
   <si>
     <t>Column Heading</t>
+  </si>
+  <si>
+    <t>LiveRoof Ontario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether the data is available to be share publically. The current data labelled as "no" can be used internally or only maps. </t>
+  </si>
+  <si>
+    <t>Stonecrest School</t>
+  </si>
+  <si>
+    <t>Brampton City Hall</t>
+  </si>
+  <si>
+    <t>Peel Memorial Hospital</t>
+  </si>
+  <si>
+    <t>Creditview Park amenity</t>
+  </si>
+  <si>
+    <t>Erin Oaks Kids</t>
+  </si>
+  <si>
+    <t>Mississauga Gateway Phase 2</t>
+  </si>
+  <si>
+    <t>UTM Instructional Centre</t>
+  </si>
+  <si>
+    <t>Burnhamthorpe Library</t>
+  </si>
+  <si>
+    <t>Celebration Square</t>
+  </si>
+  <si>
+    <t>Karl Stortz Endoscopy</t>
+  </si>
+  <si>
+    <t>EMS 106</t>
+  </si>
+  <si>
+    <t>UTM Innovation Bldg</t>
+  </si>
+  <si>
+    <t>UTM North Building</t>
+  </si>
+  <si>
+    <t>Spectrum Square</t>
+  </si>
+  <si>
+    <t>Wolfedale Yard</t>
+  </si>
+  <si>
+    <t>Grand Park Phase 2</t>
+  </si>
+  <si>
+    <t>Oak Ridges Community Centre</t>
+  </si>
+  <si>
+    <t>Vaughan Metro Centre</t>
+  </si>
+  <si>
+    <t>Chris Hadfield Public School</t>
+  </si>
+  <si>
+    <t>Brooklin Secondary School</t>
+  </si>
+  <si>
+    <t>Southeast Collectors York Durham Region</t>
   </si>
 </sst>
 </file>
@@ -2533,11 +2599,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I867"/>
+  <dimension ref="A1:I889"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <pane ySplit="1" topLeftCell="A874" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F881" sqref="F881"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23612,7 +23678,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="865" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="865" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A865" t="s">
         <v>714</v>
       </c>
@@ -23629,7 +23695,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="866" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="866" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
         <v>714</v>
       </c>
@@ -23646,7 +23712,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="867" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="867" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
         <v>714</v>
       </c>
@@ -23661,6 +23727,563 @@
       </c>
       <c r="E867" t="s">
         <v>715</v>
+      </c>
+    </row>
+    <row r="868" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A868" t="s">
+        <v>535</v>
+      </c>
+      <c r="B868">
+        <v>45.435961900000002</v>
+      </c>
+      <c r="C868">
+        <v>-76.117230000000006</v>
+      </c>
+      <c r="D868" t="s">
+        <v>536</v>
+      </c>
+      <c r="E868" t="s">
+        <v>726</v>
+      </c>
+      <c r="G868" t="s">
+        <v>728</v>
+      </c>
+      <c r="H868">
+        <v>2016</v>
+      </c>
+      <c r="I868">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="869" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A869" t="s">
+        <v>535</v>
+      </c>
+      <c r="B869">
+        <v>43.684890199999998</v>
+      </c>
+      <c r="C869">
+        <v>-79.761741700000002</v>
+      </c>
+      <c r="D869" t="s">
+        <v>536</v>
+      </c>
+      <c r="E869" t="s">
+        <v>726</v>
+      </c>
+      <c r="G869" t="s">
+        <v>729</v>
+      </c>
+      <c r="H869">
+        <v>2015</v>
+      </c>
+      <c r="I869">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="870" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A870" t="s">
+        <v>535</v>
+      </c>
+      <c r="B870">
+        <v>43.690464900000002</v>
+      </c>
+      <c r="C870">
+        <v>-79.753609999999995</v>
+      </c>
+      <c r="D870" t="s">
+        <v>536</v>
+      </c>
+      <c r="E870" t="s">
+        <v>726</v>
+      </c>
+      <c r="G870" t="s">
+        <v>730</v>
+      </c>
+      <c r="H870">
+        <v>2016</v>
+      </c>
+      <c r="I870">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="871" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A871" t="s">
+        <v>535</v>
+      </c>
+      <c r="B871">
+        <v>43.684757699999999</v>
+      </c>
+      <c r="C871">
+        <v>-79.836149300000002</v>
+      </c>
+      <c r="D871" t="s">
+        <v>536</v>
+      </c>
+      <c r="E871" t="s">
+        <v>726</v>
+      </c>
+      <c r="G871" t="s">
+        <v>731</v>
+      </c>
+      <c r="H871">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="872" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A872" t="s">
+        <v>535</v>
+      </c>
+      <c r="B872">
+        <v>43.783894099999998</v>
+      </c>
+      <c r="C872">
+        <v>-79.702034999999995</v>
+      </c>
+      <c r="D872" t="s">
+        <v>536</v>
+      </c>
+      <c r="E872" t="s">
+        <v>726</v>
+      </c>
+      <c r="G872" t="s">
+        <v>732</v>
+      </c>
+      <c r="H872">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="873" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A873" t="s">
+        <v>535</v>
+      </c>
+      <c r="B873">
+        <v>43.519468699999997</v>
+      </c>
+      <c r="C873">
+        <v>-79.689790000000002</v>
+      </c>
+      <c r="D873" t="s">
+        <v>536</v>
+      </c>
+      <c r="E873" t="s">
+        <v>726</v>
+      </c>
+      <c r="G873" t="s">
+        <v>732</v>
+      </c>
+      <c r="H873">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="874" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A874" t="s">
+        <v>535</v>
+      </c>
+      <c r="B874">
+        <v>43.656573399999999</v>
+      </c>
+      <c r="C874">
+        <v>-79.617393500000006</v>
+      </c>
+      <c r="D874" t="s">
+        <v>536</v>
+      </c>
+      <c r="E874" t="s">
+        <v>726</v>
+      </c>
+      <c r="G874" t="s">
+        <v>733</v>
+      </c>
+      <c r="H874">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="875" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A875" t="s">
+        <v>535</v>
+      </c>
+      <c r="B875">
+        <v>43.5512151</v>
+      </c>
+      <c r="C875">
+        <v>-79.664670000000001</v>
+      </c>
+      <c r="D875" t="s">
+        <v>536</v>
+      </c>
+      <c r="E875" t="s">
+        <v>726</v>
+      </c>
+      <c r="G875" t="s">
+        <v>734</v>
+      </c>
+      <c r="H875">
+        <v>2010</v>
+      </c>
+      <c r="I875">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="876" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A876" t="s">
+        <v>535</v>
+      </c>
+      <c r="B876">
+        <v>43.621042899999999</v>
+      </c>
+      <c r="C876">
+        <v>-79.605193</v>
+      </c>
+      <c r="D876" t="s">
+        <v>536</v>
+      </c>
+      <c r="E876" t="s">
+        <v>726</v>
+      </c>
+      <c r="G876" t="s">
+        <v>735</v>
+      </c>
+      <c r="H876">
+        <v>2011</v>
+      </c>
+      <c r="I876">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="877" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A877" t="s">
+        <v>535</v>
+      </c>
+      <c r="B877">
+        <v>43.587900300000001</v>
+      </c>
+      <c r="C877">
+        <v>-79.644808999999995</v>
+      </c>
+      <c r="D877" t="s">
+        <v>536</v>
+      </c>
+      <c r="E877" t="s">
+        <v>726</v>
+      </c>
+      <c r="G877" t="s">
+        <v>736</v>
+      </c>
+      <c r="H877">
+        <v>2011</v>
+      </c>
+      <c r="I877">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="878" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A878" t="s">
+        <v>535</v>
+      </c>
+      <c r="B878">
+        <v>43.598221799999997</v>
+      </c>
+      <c r="C878">
+        <v>-79.7698161</v>
+      </c>
+      <c r="D878" t="s">
+        <v>536</v>
+      </c>
+      <c r="E878" t="s">
+        <v>726</v>
+      </c>
+      <c r="G878" t="s">
+        <v>737</v>
+      </c>
+      <c r="H878">
+        <v>2011</v>
+      </c>
+      <c r="I878">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="879" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A879" t="s">
+        <v>535</v>
+      </c>
+      <c r="B879">
+        <v>43.516743900000002</v>
+      </c>
+      <c r="C879">
+        <v>-79.652690000000007</v>
+      </c>
+      <c r="D879" t="s">
+        <v>536</v>
+      </c>
+      <c r="E879" t="s">
+        <v>726</v>
+      </c>
+      <c r="G879" t="s">
+        <v>738</v>
+      </c>
+      <c r="H879">
+        <v>2012</v>
+      </c>
+      <c r="I879">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="880" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A880" t="s">
+        <v>535</v>
+      </c>
+      <c r="B880">
+        <v>43.548196900000001</v>
+      </c>
+      <c r="C880">
+        <v>-79.664117000000005</v>
+      </c>
+      <c r="D880" t="s">
+        <v>536</v>
+      </c>
+      <c r="E880" t="s">
+        <v>726</v>
+      </c>
+      <c r="G880" t="s">
+        <v>739</v>
+      </c>
+      <c r="H880">
+        <v>2014</v>
+      </c>
+      <c r="I880">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="881" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A881" t="s">
+        <v>535</v>
+      </c>
+      <c r="B881">
+        <v>43.550868899999998</v>
+      </c>
+      <c r="C881">
+        <v>-79.666358099999997</v>
+      </c>
+      <c r="D881" t="s">
+        <v>536</v>
+      </c>
+      <c r="E881" t="s">
+        <v>726</v>
+      </c>
+      <c r="G881" t="s">
+        <v>740</v>
+      </c>
+      <c r="H881">
+        <v>2014</v>
+      </c>
+      <c r="I881">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="882" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A882" t="s">
+        <v>535</v>
+      </c>
+      <c r="B882">
+        <v>43.650910500000002</v>
+      </c>
+      <c r="C882">
+        <v>-79.607369000000006</v>
+      </c>
+      <c r="D882" t="s">
+        <v>536</v>
+      </c>
+      <c r="E882" t="s">
+        <v>726</v>
+      </c>
+      <c r="G882" t="s">
+        <v>741</v>
+      </c>
+      <c r="H882">
+        <v>2015</v>
+      </c>
+      <c r="I882">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="883" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A883" t="s">
+        <v>535</v>
+      </c>
+      <c r="B883">
+        <v>43.571366500000003</v>
+      </c>
+      <c r="C883">
+        <v>-79.647947000000002</v>
+      </c>
+      <c r="D883" t="s">
+        <v>536</v>
+      </c>
+      <c r="E883" t="s">
+        <v>726</v>
+      </c>
+      <c r="G883" t="s">
+        <v>742</v>
+      </c>
+      <c r="H883">
+        <v>2016</v>
+      </c>
+      <c r="I883">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="884" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A884" t="s">
+        <v>535</v>
+      </c>
+      <c r="B884">
+        <v>43.581190700000001</v>
+      </c>
+      <c r="C884">
+        <v>-79.649805700000002</v>
+      </c>
+      <c r="D884" t="s">
+        <v>536</v>
+      </c>
+      <c r="E884" t="s">
+        <v>726</v>
+      </c>
+      <c r="G884" t="s">
+        <v>743</v>
+      </c>
+      <c r="H884">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="885" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A885" t="s">
+        <v>535</v>
+      </c>
+      <c r="B885">
+        <v>43.946603799999998</v>
+      </c>
+      <c r="C885">
+        <v>-79.430668999999995</v>
+      </c>
+      <c r="D885" t="s">
+        <v>536</v>
+      </c>
+      <c r="E885" t="s">
+        <v>726</v>
+      </c>
+      <c r="G885" t="s">
+        <v>744</v>
+      </c>
+      <c r="H885">
+        <v>2012</v>
+      </c>
+      <c r="I885">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="886" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A886" t="s">
+        <v>535</v>
+      </c>
+      <c r="B886">
+        <v>43.793337600000001</v>
+      </c>
+      <c r="C886">
+        <v>-79.530349999999999</v>
+      </c>
+      <c r="D886" t="s">
+        <v>536</v>
+      </c>
+      <c r="E886" t="s">
+        <v>726</v>
+      </c>
+      <c r="G886" t="s">
+        <v>745</v>
+      </c>
+      <c r="H886">
+        <v>2016</v>
+      </c>
+      <c r="I886">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="887" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A887" t="s">
+        <v>535</v>
+      </c>
+      <c r="B887">
+        <v>43.962730899999997</v>
+      </c>
+      <c r="C887">
+        <v>-78.971650800000006</v>
+      </c>
+      <c r="D887" t="s">
+        <v>536</v>
+      </c>
+      <c r="E887" t="s">
+        <v>726</v>
+      </c>
+      <c r="G887" t="s">
+        <v>746</v>
+      </c>
+      <c r="H887">
+        <v>2013</v>
+      </c>
+      <c r="I887">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="888" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A888" t="s">
+        <v>535</v>
+      </c>
+      <c r="B888">
+        <v>43.966813700000003</v>
+      </c>
+      <c r="C888">
+        <v>-78.962114499999998</v>
+      </c>
+      <c r="D888" t="s">
+        <v>536</v>
+      </c>
+      <c r="E888" t="s">
+        <v>726</v>
+      </c>
+      <c r="G888" t="s">
+        <v>747</v>
+      </c>
+      <c r="H888">
+        <v>2015</v>
+      </c>
+      <c r="I888">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="889" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A889" t="s">
+        <v>535</v>
+      </c>
+      <c r="B889">
+        <v>43.861328200000003</v>
+      </c>
+      <c r="C889">
+        <v>-79.173032000000006</v>
+      </c>
+      <c r="D889" t="s">
+        <v>536</v>
+      </c>
+      <c r="E889" t="s">
+        <v>726</v>
+      </c>
+      <c r="G889" t="s">
+        <v>748</v>
+      </c>
+      <c r="H889">
+        <v>2014</v>
+      </c>
+      <c r="I889">
+        <v>1115</v>
       </c>
     </row>
   </sheetData>
@@ -23673,14 +24296,14 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>716</v>
@@ -23715,7 +24338,7 @@
         <v>580</v>
       </c>
       <c r="B5" t="s">
-        <v>720</v>
+        <v>727</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -23723,7 +24346,7 @@
         <v>529</v>
       </c>
       <c r="B6" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -23731,7 +24354,7 @@
         <v>716</v>
       </c>
       <c r="B7" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -23739,7 +24362,7 @@
         <v>533</v>
       </c>
       <c r="B8" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -23747,7 +24370,7 @@
         <v>531</v>
       </c>
       <c r="B9" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -23755,7 +24378,7 @@
         <v>532</v>
       </c>
       <c r="B10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
   </sheetData>

</xml_diff>